<commit_message>
adding basic map template
</commit_message>
<xml_diff>
--- a/graphic_templates/mapping_DH/mapping_DH.xlsx
+++ b/graphic_templates/mapping_DH/mapping_DH.xlsx
@@ -17,13 +17,28 @@
     <t>key</t>
   </si>
   <si>
+    <t>state</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
-    <t>state</t>
+    <t>headline</t>
   </si>
   <si>
-    <t>headline</t>
+    <t>The Headline For This Graphic</t>
+  </si>
+  <si>
+    <t>subhed</t>
+  </si>
+  <si>
+    <t>This is default text in the copytext spreadsheet for this graphic. &lt;a href="https://docs.google.com/spreadsheets/d/{{ COPY_GOOGLE_DOC_KEY }}/edit" target="_blank"&gt;Edit this spreadsheet&lt;/a&gt; (created when you added the graphic) to update the data and text. Delete any rows you don't need, and add others as needed. Don't forget to &lt;code&gt;fab update_copy:{{ slug }}&lt;/code&gt; to update the text or visit &lt;a href="http://127.0.0.1:8000/graphics/{{ slug }}/?refresh=1" target="_top"&gt;&lt;code&gt;http://127.0.0.1:8000/graphics/{{ slug }}/?refresh=1&lt;/code&gt;&lt;/a&gt; to refresh the data every time you reload the page!</t>
+  </si>
+  <si>
+    <t>footnote</t>
+  </si>
+  <si>
+    <t>source</t>
   </si>
   <si>
     <t>something</t>
@@ -32,13 +47,7 @@
     <t>another_thing</t>
   </si>
   <si>
-    <t>The Headline For This Graphic</t>
-  </si>
-  <si>
     <t>Alabama</t>
-  </si>
-  <si>
-    <t>subhed</t>
   </si>
   <si>
     <t>2</t>
@@ -48,9 +57,6 @@
   </si>
   <si>
     <t>Alaska</t>
-  </si>
-  <si>
-    <t>This is default text in the copytext spreadsheet for this graphic. &lt;a href="https://docs.google.com/spreadsheets/d/{{ COPY_GOOGLE_DOC_KEY }}/edit" target="_blank"&gt;Edit this spreadsheet&lt;/a&gt; (created when you added the graphic) to update the data and text. Delete any rows you don't need, and add others as needed. Don't forget to &lt;code&gt;fab update_copy:{{ slug }}&lt;/code&gt; to update the text or visit &lt;a href="http://127.0.0.1:8000/graphics/{{ slug }}/?refresh=1" target="_top"&gt;&lt;code&gt;http://127.0.0.1:8000/graphics/{{ slug }}/?refresh=1&lt;/code&gt;&lt;/a&gt; to refresh the data every time you reload the page!</t>
   </si>
   <si>
     <t>4</t>
@@ -104,12 +110,6 @@
     <t>1788</t>
   </si>
   <si>
-    <t>footnote</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
     <t>credit</t>
   </si>
   <si>
@@ -149,10 +149,10 @@
       <sz val="14.0"/>
     </font>
     <font>
-      <b/>
+      <sz val="14.0"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <b/>
     </font>
     <font/>
   </fonts>
@@ -187,26 +187,26 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
@@ -244,7 +244,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -272,564 +272,564 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" ht="33.0" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+    </row>
+    <row r="3" ht="33.0" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-    </row>
-    <row r="3" ht="33.0" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+    </row>
+    <row r="4" ht="33.0" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+    </row>
+    <row r="5" ht="33.0" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-    </row>
-    <row r="4" ht="33.0" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-    </row>
-    <row r="5" ht="33.0" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
     </row>
     <row r="6" ht="33.0" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
     </row>
     <row r="7" ht="33.0" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
     </row>
     <row r="8" ht="33.0" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
     </row>
     <row r="9" ht="33.0" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
     </row>
     <row r="10" ht="33.0" customHeight="1">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
     </row>
     <row r="11" ht="33.0" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
     </row>
     <row r="12" ht="33.0" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
     </row>
     <row r="13" ht="33.0" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
     </row>
     <row r="14" ht="33.0" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
     </row>
     <row r="15" ht="33.0" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
     </row>
     <row r="16" ht="33.0" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
     </row>
     <row r="17" ht="33.0" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
     </row>
     <row r="18" ht="33.0" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
     </row>
     <row r="19" ht="33.0" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
     </row>
     <row r="20" ht="33.0" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -852,114 +852,114 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
+      <c r="A1" s="6" t="s">
+        <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="9" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="9" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="9" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="9" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="s">
         <v>29</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9">

</xml_diff>